<commit_message>
letzte Korrekturen der Aufgabe 0 :whale:
</commit_message>
<xml_diff>
--- a/Aufgabe_1/Aufgabe_1.1/Tracetable_Cows_IvenIOS.xlsx
+++ b/Aufgabe_1/Aufgabe_1.1/Tracetable_Cows_IvenIOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sirivenotissieglen/Documents/GitHub/EIA2/Aufgabe_1/Aufgabe_1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FC9CF4-0166-CD40-83D7-001BC3E07CF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DE1EF6-9D80-8A4E-AA28-9EB60F370598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C524DFDA-DA53-7849-A476-803850921D06}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Spalte7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Zeile</t>
   </si>
@@ -55,16 +52,306 @@
   </si>
   <si>
     <t>Kommentar</t>
+  </si>
+  <si>
+    <r>
+      <t>number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[] = [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF09885A"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF09885A"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF09885A"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>0&lt;3</t>
+  </si>
+  <si>
+    <r>
+      <t>createCall</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"m"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 2)</t>
+    </r>
+  </si>
+  <si>
+    <t>"m"</t>
+  </si>
+  <si>
+    <t>2&gt;0</t>
+  </si>
+  <si>
+    <t>2 ≠ 1 || 2 ≠ 1</t>
+  </si>
+  <si>
+    <t>"mu"</t>
+  </si>
+  <si>
+    <t>1&gt;0</t>
+  </si>
+  <si>
+    <t>1 =  1 || 1 = 1</t>
+  </si>
+  <si>
+    <t>"muh"</t>
+  </si>
+  <si>
+    <t>"muhu"</t>
+  </si>
+  <si>
+    <t>0&gt;0 X</t>
+  </si>
+  <si>
+    <t>return "muhu"</t>
+  </si>
+  <si>
+    <t>console.log("muhu")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1&lt;3 </t>
+  </si>
+  <si>
+    <r>
+      <t>createCall</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"m"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 6)</t>
+    </r>
+  </si>
+  <si>
+    <t>6&gt;0</t>
+  </si>
+  <si>
+    <t>5 ≠ 1</t>
+  </si>
+  <si>
+    <t>5&gt;0</t>
+  </si>
+  <si>
+    <t>"muu"</t>
+  </si>
+  <si>
+    <t>4&gt;0</t>
+  </si>
+  <si>
+    <t>4 ≠ 1</t>
+  </si>
+  <si>
+    <t>"muuu"</t>
+  </si>
+  <si>
+    <t>3 ≠ 1</t>
+  </si>
+  <si>
+    <t>3&gt;0</t>
+  </si>
+  <si>
+    <t>"muuuu"</t>
+  </si>
+  <si>
+    <t>2 ≠ 1</t>
+  </si>
+  <si>
+    <t>"muuuuu"</t>
+  </si>
+  <si>
+    <t>^^</t>
+  </si>
+  <si>
+    <t>"muuuuuh"</t>
+  </si>
+  <si>
+    <t>"muuuuuhu"</t>
+  </si>
+  <si>
+    <t>return"muuuuuhu"</t>
+  </si>
+  <si>
+    <t>console.log("muuuuuhu")</t>
+  </si>
+  <si>
+    <t>2&lt;3</t>
+  </si>
+  <si>
+    <t>createCall("m", 5)</t>
+  </si>
+  <si>
+    <t>0&gt;0</t>
+  </si>
+  <si>
+    <t>6 ≠ 1</t>
+  </si>
+  <si>
+    <t>"muuuuh"</t>
+  </si>
+  <si>
+    <t>"muuuuhu"</t>
+  </si>
+  <si>
+    <t>return"muuuuhu"</t>
+  </si>
+  <si>
+    <t>3&lt;3 X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF267F99"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF09885A"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF795E26"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA31515"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,7 +365,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -86,17 +373,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF8EA9DB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF8EA9DB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -110,16 +484,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5EC40EB-0772-A441-8337-776186504822}" name="Tabelle1" displayName="Tabelle1" ref="A1:H41" totalsRowShown="0">
-  <autoFilter ref="A1:H41" xr:uid="{C6AEE5A7-C6F7-894E-8AC2-8042B1032CC5}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5EC40EB-0772-A441-8337-776186504822}" name="Tabelle1" displayName="Tabelle1" ref="A1:G66" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G66" xr:uid="{C6AEE5A7-C6F7-894E-8AC2-8042B1032CC5}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{0010FA61-887D-5743-8832-4252C77A3E8D}" name="Zeile"/>
-    <tableColumn id="2" xr3:uid="{07EC9539-E9D2-FA4D-BB20-24F33FF2093F}" name="num i"/>
-    <tableColumn id="3" xr3:uid="{A064046D-5851-8145-9D65-A605C36B255A}" name="string result"/>
-    <tableColumn id="4" xr3:uid="{43345CAD-2C0F-A24D-B424-7A673730ED84}" name="String _start"/>
-    <tableColumn id="5" xr3:uid="{E410BD7B-EF6E-794F-89FF-06C64087EBF4}" name="num _length"/>
-    <tableColumn id="6" xr3:uid="{6DB8F798-69D7-3042-AFE2-DC2424C90557}" name="num k"/>
-    <tableColumn id="7" xr3:uid="{CFB5BFBD-EA82-8A48-B834-C3545BF813C1}" name="Spalte7"/>
+    <tableColumn id="2" xr3:uid="{07EC9539-E9D2-FA4D-BB20-24F33FF2093F}" name="num i" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A064046D-5851-8145-9D65-A605C36B255A}" name="string result" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{43345CAD-2C0F-A24D-B424-7A673730ED84}" name="String _start" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E410BD7B-EF6E-794F-89FF-06C64087EBF4}" name="num _length" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{6DB8F798-69D7-3042-AFE2-DC2424C90557}" name="num k" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{779B0BF5-78EC-1E43-8920-C2B16BD1B1F9}" name="Kommentar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -423,123 +796,991 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0863776C-B97B-D14B-91A9-738F27EA91DE}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="6" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="60.1640625" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <v>6</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>10</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>11</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>14</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3">
+        <v>5</v>
+      </c>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3">
+        <v>5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3">
+        <v>4</v>
+      </c>
+      <c r="G49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>12</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>9</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>12</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3">
+        <v>2</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>12</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
+      <c r="G58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>11</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>9</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>14</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>4</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="9">
+        <v>5</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>3</v>
+      </c>
+      <c r="B66" s="6">
+        <v>3</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
korrektur 1.1 und konsol ausgabe des browsers bestätigt.
</commit_message>
<xml_diff>
--- a/Aufgabe_1/Aufgabe_1.1/Tracetable_Cows_IvenIOS.xlsx
+++ b/Aufgabe_1/Aufgabe_1.1/Tracetable_Cows_IvenIOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sirivenotissieglen/Documents/GitHub/EIA2/Aufgabe_1/Aufgabe_1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD33C8FE-1CFD-E54C-B768-ADD5C8B69B8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18049611-8354-CB42-8043-5EC3BAD14AC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="6000" windowWidth="28800" windowHeight="16680" xr2:uid="{C524DFDA-DA53-7849-A476-803850921D06}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{C524DFDA-DA53-7849-A476-803850921D06}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Zeile</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>5 ≠  1 || 5 ≠ 2,5</t>
+  </si>
+  <si>
+    <t>Dies Bestätig sich auch in der Ausgabe der Konsole im Browser</t>
   </si>
 </sst>
 </file>
@@ -840,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0863776C-B97B-D14B-91A9-738F27EA91DE}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1807,7 +1810,9 @@
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>

</xml_diff>